<commit_message>
Added cgan model to directory
Put cgan model and newly generated weight file in SVM directory so model can be loaded by SVM classifier
</commit_message>
<xml_diff>
--- a/AUD_SUVR_wb_cingulate.xlsx
+++ b/AUD_SUVR_wb_cingulate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dagne\Desktop\AUD_study\Catalyst_GAN\Catalysis_cGAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09D7EBD-A10A-4BC4-8D95-1653FFDF2DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9558DE-9F39-4250-85DD-1F0566A3C61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5520" yWindow="3795" windowWidth="14865" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,5 +1376,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>